<commit_message>
RDM-2226 Fix variable name.
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V33_RDM-2226.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V33_RDM-2226.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-14060" yWindow="-28340" windowWidth="51200" windowHeight="28340" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-5640" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -16101,7 +16101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
@@ -16793,8 +16793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>